<commit_message>
Changed warnings to an Object.
</commit_message>
<xml_diff>
--- a/WarningTemplate.xlsx
+++ b/WarningTemplate.xlsx
@@ -24,18 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>CPF</t>
-  </si>
-  <si>
-    <t>Nome</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>AVISOS REFERENTES A 04/2020</t>
   </si>
   <si>
-    <t>Aviso</t>
+    <t>Aviso/Erro</t>
+  </si>
+  <si>
+    <t>Identificador</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Detalhe</t>
   </si>
 </sst>
 </file>
@@ -123,7 +129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -132,11 +138,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -422,42 +427,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="55.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="154.28515625" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="16.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="72.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="70" style="4" customWidth="1"/>
+    <col min="5" max="5" width="55.5703125" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="3" spans="1:3" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>